<commit_message>
A tester, 100% ça fonctionne
</commit_message>
<xml_diff>
--- a/Calcul prevision.xlsx
+++ b/Calcul prevision.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Flavien\Desktop\Perceptron_network\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6BE20D0-B999-46A8-B686-6FECCA7DF508}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5895F03-7CB6-4140-8349-221D31B6A69D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="12800" yWindow="0" windowWidth="12800" windowHeight="15400" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -56,9 +56,6 @@
     <t>res_mul = input * weight(index)</t>
   </si>
   <si>
-    <t>res_sum(hexa32bits)</t>
-  </si>
-  <si>
     <t>0x0000 0000</t>
   </si>
   <si>
@@ -92,13 +89,16 @@
     <t>res_mul_64 (hexa64bits)</t>
   </si>
   <si>
-    <t>res_mul_32 (hexa64bits)</t>
-  </si>
-  <si>
     <t>0x1000 0000</t>
   </si>
   <si>
     <t>0xA000 0000</t>
+  </si>
+  <si>
+    <t>B = res_mul_32 (hexa64bits)</t>
+  </si>
+  <si>
+    <t>A = res_sum(hexa32bits)</t>
   </si>
 </sst>
 </file>
@@ -421,8 +421,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H7"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="H1" sqref="H1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -448,16 +448,16 @@
         <v>5</v>
       </c>
       <c r="E1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="G1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H1" t="s">
-        <v>6</v>
+        <v>20</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.35">
@@ -478,7 +478,7 @@
         <v>0</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.35">
@@ -496,17 +496,17 @@
         <v>1.5</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G3">
         <f>G2+D3</f>
         <v>1.5</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.35">
@@ -524,17 +524,17 @@
         <v>0.5</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="G4">
         <f>G3+D4</f>
         <v>2</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.35">
@@ -552,17 +552,17 @@
         <v>-1</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="G5">
         <f>G4+D5</f>
         <v>1</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.35">
@@ -580,17 +580,17 @@
         <v>2</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G6">
         <f>G5+D6</f>
         <v>3</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
Modification python pour taille réglable
</commit_message>
<xml_diff>
--- a/Calcul prevision.xlsx
+++ b/Calcul prevision.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Flavien\Desktop\Perceptron_network\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\flavi\Desktop\Perceptron_network\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5895F03-7CB6-4140-8349-221D31B6A69D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51C61939-8B1E-4712-91DA-335C6803FF75}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12800" yWindow="0" windowWidth="12800" windowHeight="15400" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -95,10 +95,10 @@
     <t>0xA000 0000</t>
   </si>
   <si>
-    <t>B = res_mul_32 (hexa64bits)</t>
-  </si>
-  <si>
     <t>A = res_sum(hexa32bits)</t>
+  </si>
+  <si>
+    <t>B = res_mul_32 (hexa32bits)</t>
   </si>
 </sst>
 </file>
@@ -421,20 +421,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H7"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="H1" sqref="H1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="4" max="4" width="30.36328125" customWidth="1"/>
+    <col min="4" max="4" width="30.42578125" customWidth="1"/>
     <col min="5" max="5" width="28" customWidth="1"/>
-    <col min="6" max="6" width="28.1796875" customWidth="1"/>
-    <col min="7" max="7" width="30.26953125" customWidth="1"/>
-    <col min="8" max="8" width="29.08984375" customWidth="1"/>
+    <col min="6" max="6" width="28.140625" customWidth="1"/>
+    <col min="7" max="7" width="30.28515625" customWidth="1"/>
+    <col min="8" max="8" width="29.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -451,16 +451,16 @@
         <v>16</v>
       </c>
       <c r="F1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="G1" t="s">
         <v>12</v>
       </c>
       <c r="H1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -481,7 +481,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>0</v>
       </c>
@@ -509,7 +509,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>1</v>
       </c>
@@ -537,7 +537,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>2</v>
       </c>
@@ -565,7 +565,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>3</v>
       </c>
@@ -593,7 +593,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>4</v>
       </c>

</xml_diff>

<commit_message>
Ajout conversion inversé en hexa
</commit_message>
<xml_diff>
--- a/Calcul prevision.xlsx
+++ b/Calcul prevision.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\flavi\Desktop\Perceptron_network\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51C61939-8B1E-4712-91DA-335C6803FF75}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F35DF788-D687-41C7-A545-BFDFD2541AA5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="24">
   <si>
     <t>index</t>
   </si>
@@ -99,13 +99,22 @@
   </si>
   <si>
     <t>B = res_mul_32 (hexa32bits)</t>
+  </si>
+  <si>
+    <t>0x87C0 0000 0000 0000</t>
+  </si>
+  <si>
+    <t>0xBE00 0000</t>
+  </si>
+  <si>
+    <t>0x2200 0000</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -113,16 +122,29 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -130,17 +152,35 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Check Cell" xfId="1" builtinId="23"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -422,7 +462,7 @@
   <dimension ref="A1:H7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+      <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -434,33 +474,33 @@
     <col min="8" max="8" width="29.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:8" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G1" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="H1" t="s">
+      <c r="H1" s="2" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -520,7 +560,7 @@
         <v>1</v>
       </c>
       <c r="D4">
-        <f t="shared" ref="D4:D6" si="0">B4*C4</f>
+        <f t="shared" ref="D4:D7" si="0">B4*C4</f>
         <v>0.5</v>
       </c>
       <c r="E4" s="1" t="s">
@@ -597,8 +637,32 @@
       <c r="A7">
         <v>4</v>
       </c>
+      <c r="B7">
+        <v>-1.9375</v>
+      </c>
+      <c r="C7">
+        <v>1</v>
+      </c>
+      <c r="D7">
+        <f t="shared" si="0"/>
+        <v>-1.9375</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="G7">
+        <f>G6+D7</f>
+        <v>1.0625</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>23</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>